<commit_message>
updating respondus excel files
</commit_message>
<xml_diff>
--- a/newman/excel/StatisticsToolsRespondus.xlsx
+++ b/newman/excel/StatisticsToolsRespondus.xlsx
@@ -8,9 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan.Newman\Dropbox\github\SanJacMath.github.io\SanJacMath.github.io\newman\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483D515A-22CB-4D3D-9A77-86E940B75F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5BB658-6006-4250-8369-AAFBD4208ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="tUKASPPaeggjveXVhoXjI84zB7d9adI+z2YD9isDLGv5/GdnWmV7pPuyP0Xjzdyb8cPnzaY5pPocFoudybRfPw==" workbookSaltValue="V6T/GNF5TcReyz0qSaV16g==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="1695" windowWidth="21600" windowHeight="13380" tabRatio="769" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="769" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleStats" sheetId="1" r:id="rId1"/>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="177">
   <si>
     <t>Type sample data in the column below, and the statistics will calculate on the right</t>
   </si>
@@ -757,9 +758,6 @@
     <t>Scatterplot tool not available in Respondus</t>
   </si>
   <si>
-    <t>Usage warnings here</t>
-  </si>
-  <si>
     <t>max =</t>
   </si>
   <si>
@@ -773,11 +771,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.######"/>
-    <numFmt numFmtId="169" formatCode="0.#####"/>
+    <numFmt numFmtId="166" formatCode="0.######"/>
+    <numFmt numFmtId="167" formatCode="0.#####"/>
+    <numFmt numFmtId="168" formatCode="0.########"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -946,7 +945,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1061,9 +1060,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -1089,21 +1085,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="169" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1111,6 +1103,19 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2056,178 +2061,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>505558</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>21981</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>395654</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>14654</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="TextBox 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B18E0EAC-5F58-40B9-8AFE-DE97679CA267}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2029558" y="3260481"/>
-          <a:ext cx="5707673" cy="1897673"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Note that copy/paste is not available within</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> this web-based version of Excel</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>, so you'll need to carefully type any data</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> values to input them</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>.  For this reason, I will try to keep a manageable size for any data sets during tests.  </a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-US" sz="1400" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-          </a:br>
-          <a:br>
-            <a:rPr lang="en-US" sz="1400" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>This version of Excel may not allow you to delete multiple entries, so to clear out your input, you can backspace over individual values, or just reload the tab at the top of your web browser to have a fresh copy with all of the input cleared out, as needed.</a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-          </a:br>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
@@ -3656,7 +3489,7 @@
         <v/>
       </c>
       <c r="B4" s="39"/>
-      <c r="D4" s="53" t="s">
+      <c r="D4" s="52" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="45">
@@ -3676,7 +3509,7 @@
         <v/>
       </c>
       <c r="B5" s="39"/>
-      <c r="D5" s="53" t="s">
+      <c r="D5" s="52" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="45" t="str">
@@ -3696,7 +3529,7 @@
         <v/>
       </c>
       <c r="B6" s="39"/>
-      <c r="D6" s="53" t="s">
+      <c r="D6" s="52" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="45" t="str">
@@ -3716,7 +3549,7 @@
         <v/>
       </c>
       <c r="B7" s="39"/>
-      <c r="D7" s="53" t="s">
+      <c r="D7" s="52" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="45" t="str">
@@ -3736,7 +3569,7 @@
         <v/>
       </c>
       <c r="B8" s="39"/>
-      <c r="D8" s="53" t="s">
+      <c r="D8" s="52" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="45" t="str">
@@ -3756,8 +3589,8 @@
         <v/>
       </c>
       <c r="B9" s="39"/>
-      <c r="D9" s="54" t="s">
-        <v>177</v>
+      <c r="D9" s="53" t="s">
+        <v>176</v>
       </c>
       <c r="E9" s="45" t="str">
         <f>IF(E4=0,"",SUM(B3:B202))</f>
@@ -3776,8 +3609,8 @@
         <v/>
       </c>
       <c r="B10" s="39"/>
-      <c r="D10" s="54" t="s">
-        <v>176</v>
+      <c r="D10" s="53" t="s">
+        <v>175</v>
       </c>
       <c r="E10" s="45" t="str">
         <f>IF(E4=0,"",SUMPRODUCT(B3:B202,B3:B202))</f>
@@ -3796,7 +3629,7 @@
         <v/>
       </c>
       <c r="B11" s="39"/>
-      <c r="D11" s="55"/>
+      <c r="D11" s="54"/>
       <c r="F11" s="15" t="s">
         <v>172</v>
       </c>
@@ -3807,7 +3640,7 @@
         <v/>
       </c>
       <c r="B12" s="39"/>
-      <c r="D12" s="53" t="s">
+      <c r="D12" s="52" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="45" t="str">
@@ -3827,7 +3660,7 @@
         <v/>
       </c>
       <c r="B13" s="39"/>
-      <c r="D13" s="53" t="s">
+      <c r="D13" s="52" t="s">
         <v>19</v>
       </c>
       <c r="E13" s="45" t="str">
@@ -3848,7 +3681,7 @@
         <v/>
       </c>
       <c r="B14" s="39"/>
-      <c r="D14" s="53" t="s">
+      <c r="D14" s="52" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="45" t="str">
@@ -3868,7 +3701,7 @@
         <v/>
       </c>
       <c r="B15" s="39"/>
-      <c r="D15" s="53" t="s">
+      <c r="D15" s="52" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="45" t="str">
@@ -3889,8 +3722,8 @@
         <v/>
       </c>
       <c r="B16" s="39"/>
-      <c r="D16" s="53" t="s">
-        <v>175</v>
+      <c r="D16" s="52" t="s">
+        <v>174</v>
       </c>
       <c r="E16" s="45" t="str">
         <f>IF(E4=0,"",MAX(B3:B202))</f>
@@ -3930,9 +3763,7 @@
         <v/>
       </c>
       <c r="B20" s="39"/>
-      <c r="D20" s="15" t="s">
-        <v>174</v>
-      </c>
+      <c r="D20" s="15"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="str">
@@ -5209,7 +5040,7 @@
       <c r="B202" s="39"/>
     </row>
   </sheetData>
-  <sheetProtection sort="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="xsVfw6vqCWzhO2dpIBrwocgmhOLJv+9ZZC6xv8YnFciS1DU4SE/itP9WfGXCnvAzYs6qH0p4XznTXk9s2vW7Pw==" saltValue="X4a7bArU4BicKUFYxf7EWQ==" spinCount="100000" sheet="1" sort="0"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:B6">
     <sortCondition ref="B3:B6"/>
   </sortState>
@@ -5280,27 +5111,27 @@
       <c r="G3" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="H3" s="63" t="str">
+      <c r="H3" s="60" t="str">
         <f>IF(OR(H4&lt;&gt;"",COUNT(A3:A102)=0),"",AVERAGE(A3:A102))</f>
         <v/>
       </c>
-      <c r="I3" s="63" t="str">
+      <c r="I3" s="60" t="str">
         <f>IF(OR(H4&lt;&gt;"",COUNT(B3:B102)=0),"",AVERAGE(B3:B102))</f>
         <v/>
       </c>
-      <c r="J3" s="63" t="str">
+      <c r="J3" s="60" t="str">
         <f>IF(OR(H4&lt;&gt;"",COUNT(C3:C102)=0),"",AVERAGE(C3:C102))</f>
         <v/>
       </c>
-      <c r="K3" s="63" t="str">
+      <c r="K3" s="60" t="str">
         <f>IF(OR(H4&lt;&gt;"",COUNT(D3:D102)=0),"",AVERAGE(D3:D102))</f>
         <v/>
       </c>
-      <c r="L3" s="63" t="str">
+      <c r="L3" s="60" t="str">
         <f>IF(OR(H4&lt;&gt;"",COUNT(E3:E102)=0),"",AVERAGE(E3:E102))</f>
         <v/>
       </c>
-      <c r="M3" s="63" t="str">
+      <c r="M3" s="60" t="str">
         <f>IF(OR(H4&lt;&gt;"",COUNT(F3:F102)=0),"",AVERAGE(F3:F102))</f>
         <v/>
       </c>
@@ -5359,31 +5190,31 @@
       <c r="G6" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="H6" s="46" t="str">
+      <c r="H6" s="66" t="str">
         <f>IF(H4&lt;&gt;"","",COUNT(H3:M3)-1)</f>
         <v/>
       </c>
-      <c r="I6" s="62" t="str">
+      <c r="I6" s="59" t="str">
         <f>IF(H4&lt;&gt;"","",IF(COUNT(A3:A102)=0,0,COUNT(A3:A102)*(AVERAGE(A3:A102)-AVERAGE(A3:F102))^2)+IF(COUNT(B3:B102)=0,0,COUNT(B3:B102)*(AVERAGE(B3:B102)-AVERAGE(A3:F102))^2)+IF(COUNT(C3:C102)=0,0,COUNT(C3:C102)*(AVERAGE(C3:C102)-AVERAGE(A3:F102))^2)+IF(COUNT(D3:D102)=0,0,COUNT(D3:D102)*(AVERAGE(D3:D102)-AVERAGE(A3:F102))^2)+IF(COUNT(E3:E102)=0,0,COUNT(E3:E102)*(AVERAGE(E3:E102)-AVERAGE(A3:F102))^2)+IF(COUNT(F3:F102)=0,0,COUNT(F3:F102)*(AVERAGE(F3:F102)-AVERAGE(A3:F102))^2))</f>
         <v/>
       </c>
-      <c r="J6" s="62" t="str">
+      <c r="J6" s="59" t="str">
         <f>IF(H4&lt;&gt;"","",I6/H6)</f>
         <v/>
       </c>
-      <c r="K6" s="62" t="str">
+      <c r="K6" s="59" t="str">
         <f>IF(H4&lt;&gt;"","",J6/J7)</f>
         <v/>
       </c>
-      <c r="L6" s="62" t="str">
+      <c r="L6" s="59" t="str">
         <f>IF(H4&lt;&gt;"","",FDIST(K6,H6,H7))</f>
         <v/>
       </c>
       <c r="M6" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="N6" s="47"/>
-      <c r="O6" s="62" t="str">
+      <c r="N6" s="46"/>
+      <c r="O6" s="59" t="str">
         <f>IF(H4&lt;&gt;"","",IF(ISBLANK(N6),"",IF(OR(NOT(ISNUMBER(N6)),N6&gt;=1,N6&lt;=0),"",FINV(N6,H6,H7))))</f>
         <v/>
       </c>
@@ -5401,15 +5232,15 @@
       <c r="G7" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="H7" s="46" t="str">
+      <c r="H7" s="66" t="str">
         <f>IF(H4&lt;&gt;"","",COUNT(A3:F102)-COUNT(H3:M3))</f>
         <v/>
       </c>
-      <c r="I7" s="62" t="str">
+      <c r="I7" s="59" t="str">
         <f>IF(H4&lt;&gt;"","",IF(COUNT(A3:A102)=0,0,(COUNT(A3:A102)-1)*(_xlfn.STDEV.S(A3:A102))^2)+IF(COUNT(B3:B102)=0,0,(COUNT(B3:B102)-1)*(_xlfn.STDEV.S(B3:B102))^2)+IF(COUNT(C3:C102)=0,0,(COUNT(C3:C102)-1)*(_xlfn.STDEV.S(C3:C102))^2)+IF(COUNT(D3:D102)=0,0,(COUNT(D3:D102)-1)*(_xlfn.STDEV.S(D3:D102))^2)+IF(COUNT(E3:E102)=0,0,(COUNT(E3:E102)-1)*(_xlfn.STDEV.S(E3:E102))^2)+IF(COUNT(F3:F102)=0,0,(COUNT(F3:F102)-1)*(_xlfn.STDEV.S(F3:F102))^2))</f>
         <v/>
       </c>
-      <c r="J7" s="62" t="str">
+      <c r="J7" s="59" t="str">
         <f>IF(H4&lt;&gt;"","",I7/H7)</f>
         <v/>
       </c>
@@ -5432,11 +5263,11 @@
       <c r="G8" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="H8" s="46" t="str">
+      <c r="H8" s="66" t="str">
         <f>IF(H4&lt;&gt;"","",H6+H7)</f>
         <v/>
       </c>
-      <c r="I8" s="62" t="str">
+      <c r="I8" s="59" t="str">
         <f>IF(H4&lt;&gt;"","",I6+I7)</f>
         <v/>
       </c>
@@ -6287,6 +6118,7 @@
       <c r="F102" s="39"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="l/bke3v5WNoexdLQAjaRzNHYFjkJRnJRC+DQa9RMSxgntYKT6FTL+TNCbWCf5yuFPvZLzKqatdPHTCL55mv7xA==" saltValue="Caf/2wjvW7xyH6SEwlLKgA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -6386,10 +6218,10 @@
         <f t="shared" ref="F4:F67" si="2">IF(ISNUMBER(A4),E4/C4,"")</f>
         <v/>
       </c>
-      <c r="H4" s="54" t="s">
+      <c r="H4" s="53" t="s">
         <v>164</v>
       </c>
-      <c r="I4" s="65" t="str">
+      <c r="I4" s="62" t="str">
         <f>IF(MAX(A3:A102)=0,"",IF(AND(MAX(A3:A102)=COUNT(B3:B102),MAX(A3:A102)=COUNT(C3:C102)),SUM(F3:F102),"Input Error"))</f>
         <v/>
       </c>
@@ -6420,7 +6252,7 @@
         <v/>
       </c>
       <c r="G5" s="6"/>
-      <c r="H5" s="54" t="s">
+      <c r="H5" s="53" t="s">
         <v>166</v>
       </c>
       <c r="I5" s="37" t="str">
@@ -6451,10 +6283,10 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H6" s="52" t="s">
+      <c r="H6" s="51" t="s">
         <v>167</v>
       </c>
-      <c r="I6" s="57" t="str">
+      <c r="I6" s="56" t="str">
         <f>IF(OR(I4="",I4="Input Error"),"",CHIDIST(I4,I5))</f>
         <v/>
       </c>
@@ -6506,15 +6338,13 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H8" s="64" t="s">
+      <c r="H8" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="I8" s="41">
-        <v>0.05</v>
-      </c>
+      <c r="I8" s="41"/>
       <c r="J8" s="16" t="str">
         <f>IF(ISBLANK(I8),"",IF(OR(NOT(ISNUMBER(I8)),I8&gt;=1,I8&lt;=0),"α must be between 0 and 1"," "))</f>
-        <v xml:space="preserve"> </v>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -6536,7 +6366,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H9" s="52" t="s">
+      <c r="H9" s="51" t="s">
         <v>170</v>
       </c>
       <c r="I9" s="44" t="str">
@@ -8397,6 +8227,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="2UfNcgQANMSLzrj3sIQ+RQloSqKpD/uPzlS/kFWvnkM4/i5LlOzHUz9jHuFdYsssfSo6tfv1zfytRLOf6oaATg==" saltValue="BbJUVxo2nUWhEXoPyjUxsw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -8458,7 +8289,7 @@
       </c>
       <c r="B4" s="39"/>
       <c r="C4" s="39"/>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="52" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="38">
@@ -8479,14 +8310,14 @@
       </c>
       <c r="B5" s="39"/>
       <c r="C5" s="39"/>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="52" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="38" t="str">
         <f>IF(OR(F4="Input Error",F4&lt;2),"",AVERAGE(B3:B102))</f>
         <v/>
       </c>
-      <c r="G5" s="48" t="s">
+      <c r="G5" s="47" t="s">
         <v>172</v>
       </c>
       <c r="H5" s="6" t="s">
@@ -8500,7 +8331,7 @@
       </c>
       <c r="B6" s="39"/>
       <c r="C6" s="39"/>
-      <c r="E6" s="53" t="s">
+      <c r="E6" s="52" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="38" t="str">
@@ -8521,14 +8352,14 @@
       </c>
       <c r="B7" s="39"/>
       <c r="C7" s="39"/>
-      <c r="E7" s="53" t="s">
+      <c r="E7" s="52" t="s">
         <v>31</v>
       </c>
       <c r="F7" s="38" t="str">
         <f>IF(OR(F4="Input Error",F4&lt;2),"",CORREL(B3:B102,C3:C102))</f>
         <v/>
       </c>
-      <c r="G7" s="48" t="s">
+      <c r="G7" s="47" t="s">
         <v>172</v>
       </c>
       <c r="H7" s="6" t="s">
@@ -8542,7 +8373,7 @@
       </c>
       <c r="B8" s="39"/>
       <c r="C8" s="39"/>
-      <c r="E8" s="53" t="s">
+      <c r="E8" s="52" t="s">
         <v>33</v>
       </c>
       <c r="F8" s="38" t="str">
@@ -8578,7 +8409,7 @@
       </c>
       <c r="B10" s="39"/>
       <c r="C10" s="39"/>
-      <c r="E10" s="53" t="s">
+      <c r="E10" s="52" t="s">
         <v>36</v>
       </c>
       <c r="F10" s="38" t="str">
@@ -8599,7 +8430,7 @@
       </c>
       <c r="B11" s="39"/>
       <c r="C11" s="39"/>
-      <c r="E11" s="53" t="s">
+      <c r="E11" s="52" t="s">
         <v>38</v>
       </c>
       <c r="F11" s="38" t="str">
@@ -9354,6 +9185,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="xxhwVTZzO6CWwKJ1Z+QapGN7nqo+90rZTZ5KMdUyHpmqNjAZoVFOkzAOn5xy0DOksWw0ZDr9kBPq72G4Mq3r3g==" saltValue="yHV6zUDRCG0RN8Klsc1mqQ==" spinCount="100000" sheet="1" scenarios="1" sort="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -9398,8 +9230,8 @@
         <f>IF(AND(ISNUMBER(B3),ISNUMBER(C3)),MAX(A1:A2)+1,"")</f>
         <v/>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
       <c r="D3" s="15" t="s">
         <v>172</v>
       </c>
@@ -9412,12 +9244,12 @@
         <f>IF(AND(ISNUMBER(B4),ISNUMBER(C4)),MAX(A1:A3)+1,"")</f>
         <v/>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
       <c r="D4" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="53" t="s">
         <v>42</v>
       </c>
       <c r="F4" s="38">
@@ -9436,12 +9268,12 @@
         <f>IF(AND(ISNUMBER(B5),ISNUMBER(C5)),MAX(A1:A4)+1,"")</f>
         <v/>
       </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
       <c r="D5" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="E5" s="54" t="s">
+      <c r="E5" s="53" t="s">
         <v>44</v>
       </c>
       <c r="F5" s="38">
@@ -9460,19 +9292,19 @@
         <f>IF(AND(ISNUMBER(B6),ISNUMBER(C6)),MAX(A1:A5)+1,"")</f>
         <v/>
       </c>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
       <c r="D6" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="E6" s="54" t="s">
+      <c r="E6" s="53" t="s">
         <v>46</v>
       </c>
       <c r="F6" s="38">
         <f>IF(AND(COUNT(A3:A102)=COUNT(B3:B102),COUNT(A3:A102)=COUNT(C3:C102)),SQRT(SUMPRODUCT(B3:B102,B3:B102,C3:C102)-(SUMPRODUCT(B3:B102,C3:C102))^2),"")</f>
         <v>0</v>
       </c>
-      <c r="G6" s="48" t="s">
+      <c r="G6" s="47" t="s">
         <v>172</v>
       </c>
       <c r="H6" s="6" t="s">
@@ -9484,8 +9316,8 @@
         <f>IF(AND(ISNUMBER(B7),ISNUMBER(C7)),MAX(A1:A6)+1,"")</f>
         <v/>
       </c>
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
+      <c r="B7" s="64"/>
+      <c r="C7" s="64"/>
       <c r="D7" s="15" t="s">
         <v>172</v>
       </c>
@@ -9495,8 +9327,8 @@
         <f>IF(AND(ISNUMBER(B8),ISNUMBER(C8)),MAX(A1:A7)+1,"")</f>
         <v/>
       </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
       <c r="D8" s="15" t="s">
         <v>172</v>
       </c>
@@ -9506,8 +9338,8 @@
         <f>IF(AND(ISNUMBER(B9),ISNUMBER(C9)),MAX(A1:A8)+1,"")</f>
         <v/>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
+      <c r="B9" s="64"/>
+      <c r="C9" s="64"/>
       <c r="D9" s="15" t="s">
         <v>172</v>
       </c>
@@ -9517,8 +9349,8 @@
         <f>IF(AND(ISNUMBER(B10),ISNUMBER(C10)),MAX(A1:A9)+1,"")</f>
         <v/>
       </c>
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="64"/>
       <c r="D10" s="15" t="s">
         <v>172</v>
       </c>
@@ -9528,8 +9360,8 @@
         <f>IF(AND(ISNUMBER(B11),ISNUMBER(C11)),MAX(A1:A10)+1,"")</f>
         <v/>
       </c>
-      <c r="B11" s="47"/>
-      <c r="C11" s="47"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="64"/>
       <c r="D11" s="15" t="s">
         <v>172</v>
       </c>
@@ -9539,8 +9371,8 @@
         <f>IF(AND(ISNUMBER(B12),ISNUMBER(C12)),MAX(A1:A11)+1,"")</f>
         <v/>
       </c>
-      <c r="B12" s="47"/>
-      <c r="C12" s="47"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="64"/>
       <c r="D12" s="15" t="s">
         <v>172</v>
       </c>
@@ -9550,8 +9382,8 @@
         <f>IF(AND(ISNUMBER(B13),ISNUMBER(C13)),MAX(A1:A12)+1,"")</f>
         <v/>
       </c>
-      <c r="B13" s="47"/>
-      <c r="C13" s="47"/>
+      <c r="B13" s="64"/>
+      <c r="C13" s="64"/>
       <c r="D13" s="15" t="s">
         <v>172</v>
       </c>
@@ -9561,8 +9393,8 @@
         <f>IF(AND(ISNUMBER(B14),ISNUMBER(C14)),MAX(A1:A13)+1,"")</f>
         <v/>
       </c>
-      <c r="B14" s="47"/>
-      <c r="C14" s="47"/>
+      <c r="B14" s="64"/>
+      <c r="C14" s="64"/>
       <c r="D14" s="15" t="s">
         <v>172</v>
       </c>
@@ -9572,8 +9404,8 @@
         <f>IF(AND(ISNUMBER(B15),ISNUMBER(C15)),MAX(A1:A14)+1,"")</f>
         <v/>
       </c>
-      <c r="B15" s="47"/>
-      <c r="C15" s="47"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="64"/>
       <c r="D15" s="15" t="s">
         <v>172</v>
       </c>
@@ -9583,8 +9415,8 @@
         <f>IF(AND(ISNUMBER(B16),ISNUMBER(C16)),MAX(A1:A15)+1,"")</f>
         <v/>
       </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="47"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="64"/>
       <c r="D16" s="15" t="s">
         <v>172</v>
       </c>
@@ -9594,8 +9426,8 @@
         <f>IF(AND(ISNUMBER(B17),ISNUMBER(C17)),MAX(A1:A16)+1,"")</f>
         <v/>
       </c>
-      <c r="B17" s="47"/>
-      <c r="C17" s="47"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="64"/>
       <c r="D17" s="15" t="s">
         <v>172</v>
       </c>
@@ -9605,8 +9437,8 @@
         <f>IF(AND(ISNUMBER(B18),ISNUMBER(C18)),MAX(A1:A17)+1,"")</f>
         <v/>
       </c>
-      <c r="B18" s="47"/>
-      <c r="C18" s="47"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="64"/>
       <c r="D18" s="15" t="s">
         <v>172</v>
       </c>
@@ -9616,8 +9448,8 @@
         <f>IF(AND(ISNUMBER(B19),ISNUMBER(C19)),MAX(A1:A18)+1,"")</f>
         <v/>
       </c>
-      <c r="B19" s="47"/>
-      <c r="C19" s="47"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="64"/>
       <c r="D19" s="15" t="s">
         <v>172</v>
       </c>
@@ -9627,8 +9459,8 @@
         <f>IF(AND(ISNUMBER(B20),ISNUMBER(C20)),MAX(A1:A19)+1,"")</f>
         <v/>
       </c>
-      <c r="B20" s="47"/>
-      <c r="C20" s="47"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="64"/>
       <c r="D20" s="15" t="s">
         <v>172</v>
       </c>
@@ -9638,8 +9470,8 @@
         <f>IF(AND(ISNUMBER(B21),ISNUMBER(C21)),MAX(A1:A20)+1,"")</f>
         <v/>
       </c>
-      <c r="B21" s="47"/>
-      <c r="C21" s="47"/>
+      <c r="B21" s="64"/>
+      <c r="C21" s="64"/>
       <c r="D21" s="15" t="s">
         <v>172</v>
       </c>
@@ -9649,8 +9481,8 @@
         <f>IF(AND(ISNUMBER(B22),ISNUMBER(C22)),MAX(A1:A21)+1,"")</f>
         <v/>
       </c>
-      <c r="B22" s="47"/>
-      <c r="C22" s="47"/>
+      <c r="B22" s="64"/>
+      <c r="C22" s="64"/>
       <c r="D22" s="15" t="s">
         <v>172</v>
       </c>
@@ -9660,8 +9492,8 @@
         <f>IF(AND(ISNUMBER(B23),ISNUMBER(C23)),MAX(A1:A22)+1,"")</f>
         <v/>
       </c>
-      <c r="B23" s="47"/>
-      <c r="C23" s="47"/>
+      <c r="B23" s="64"/>
+      <c r="C23" s="64"/>
       <c r="D23" s="15" t="s">
         <v>172</v>
       </c>
@@ -9671,8 +9503,8 @@
         <f>IF(AND(ISNUMBER(B24),ISNUMBER(C24)),MAX(A1:A23)+1,"")</f>
         <v/>
       </c>
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="64"/>
       <c r="D24" s="15" t="s">
         <v>172</v>
       </c>
@@ -9682,8 +9514,8 @@
         <f>IF(AND(ISNUMBER(B25),ISNUMBER(C25)),MAX(A1:A24)+1,"")</f>
         <v/>
       </c>
-      <c r="B25" s="47"/>
-      <c r="C25" s="47"/>
+      <c r="B25" s="64"/>
+      <c r="C25" s="64"/>
       <c r="D25" s="15" t="s">
         <v>172</v>
       </c>
@@ -9693,8 +9525,8 @@
         <f>IF(AND(ISNUMBER(B26),ISNUMBER(C26)),MAX(A1:A25)+1,"")</f>
         <v/>
       </c>
-      <c r="B26" s="47"/>
-      <c r="C26" s="47"/>
+      <c r="B26" s="64"/>
+      <c r="C26" s="64"/>
       <c r="D26" s="15" t="s">
         <v>172</v>
       </c>
@@ -9704,8 +9536,8 @@
         <f>IF(AND(ISNUMBER(B27),ISNUMBER(C27)),MAX(A1:A26)+1,"")</f>
         <v/>
       </c>
-      <c r="B27" s="47"/>
-      <c r="C27" s="47"/>
+      <c r="B27" s="64"/>
+      <c r="C27" s="64"/>
       <c r="D27" s="15" t="s">
         <v>172</v>
       </c>
@@ -9715,8 +9547,8 @@
         <f>IF(AND(ISNUMBER(B28),ISNUMBER(C28)),MAX(A1:A27)+1,"")</f>
         <v/>
       </c>
-      <c r="B28" s="47"/>
-      <c r="C28" s="47"/>
+      <c r="B28" s="64"/>
+      <c r="C28" s="64"/>
       <c r="D28" s="15" t="s">
         <v>172</v>
       </c>
@@ -9726,8 +9558,8 @@
         <f>IF(AND(ISNUMBER(B29),ISNUMBER(C29)),MAX(A1:A28)+1,"")</f>
         <v/>
       </c>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
+      <c r="B29" s="64"/>
+      <c r="C29" s="64"/>
       <c r="D29" s="15" t="s">
         <v>172</v>
       </c>
@@ -9737,8 +9569,8 @@
         <f>IF(AND(ISNUMBER(B30),ISNUMBER(C30)),MAX(A1:A29)+1,"")</f>
         <v/>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
+      <c r="B30" s="64"/>
+      <c r="C30" s="64"/>
       <c r="D30" s="15" t="s">
         <v>172</v>
       </c>
@@ -9748,8 +9580,8 @@
         <f>IF(AND(ISNUMBER(B31),ISNUMBER(C31)),MAX(A1:A30)+1,"")</f>
         <v/>
       </c>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47"/>
+      <c r="B31" s="64"/>
+      <c r="C31" s="64"/>
       <c r="D31" s="15" t="s">
         <v>172</v>
       </c>
@@ -9759,8 +9591,8 @@
         <f>IF(AND(ISNUMBER(B32),ISNUMBER(C32)),MAX(A1:A31)+1,"")</f>
         <v/>
       </c>
-      <c r="B32" s="47"/>
-      <c r="C32" s="47"/>
+      <c r="B32" s="64"/>
+      <c r="C32" s="64"/>
       <c r="D32" s="15" t="s">
         <v>172</v>
       </c>
@@ -9770,8 +9602,8 @@
         <f>IF(AND(ISNUMBER(B33),ISNUMBER(C33)),MAX(A1:A32)+1,"")</f>
         <v/>
       </c>
-      <c r="B33" s="47"/>
-      <c r="C33" s="47"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="64"/>
       <c r="D33" s="15" t="s">
         <v>172</v>
       </c>
@@ -9781,8 +9613,8 @@
         <f>IF(AND(ISNUMBER(B34),ISNUMBER(C34)),MAX(A1:A33)+1,"")</f>
         <v/>
       </c>
-      <c r="B34" s="47"/>
-      <c r="C34" s="47"/>
+      <c r="B34" s="64"/>
+      <c r="C34" s="64"/>
       <c r="D34" s="15" t="s">
         <v>172</v>
       </c>
@@ -9792,8 +9624,8 @@
         <f>IF(AND(ISNUMBER(B35),ISNUMBER(C35)),MAX(A1:A34)+1,"")</f>
         <v/>
       </c>
-      <c r="B35" s="47"/>
-      <c r="C35" s="47"/>
+      <c r="B35" s="64"/>
+      <c r="C35" s="64"/>
       <c r="D35" s="15" t="s">
         <v>172</v>
       </c>
@@ -9803,8 +9635,8 @@
         <f>IF(AND(ISNUMBER(B36),ISNUMBER(C36)),MAX(A1:A35)+1,"")</f>
         <v/>
       </c>
-      <c r="B36" s="47"/>
-      <c r="C36" s="47"/>
+      <c r="B36" s="64"/>
+      <c r="C36" s="64"/>
       <c r="D36" s="15" t="s">
         <v>172</v>
       </c>
@@ -9814,8 +9646,8 @@
         <f>IF(AND(ISNUMBER(B37),ISNUMBER(C37)),MAX(A1:A36)+1,"")</f>
         <v/>
       </c>
-      <c r="B37" s="47"/>
-      <c r="C37" s="47"/>
+      <c r="B37" s="64"/>
+      <c r="C37" s="64"/>
       <c r="D37" s="15" t="s">
         <v>172</v>
       </c>
@@ -9825,8 +9657,8 @@
         <f>IF(AND(ISNUMBER(B38),ISNUMBER(C38)),MAX(A1:A37)+1,"")</f>
         <v/>
       </c>
-      <c r="B38" s="47"/>
-      <c r="C38" s="47"/>
+      <c r="B38" s="64"/>
+      <c r="C38" s="64"/>
       <c r="D38" s="15" t="s">
         <v>172</v>
       </c>
@@ -9836,8 +9668,8 @@
         <f>IF(AND(ISNUMBER(B39),ISNUMBER(C39)),MAX(A1:A38)+1,"")</f>
         <v/>
       </c>
-      <c r="B39" s="47"/>
-      <c r="C39" s="47"/>
+      <c r="B39" s="64"/>
+      <c r="C39" s="64"/>
       <c r="D39" s="15" t="s">
         <v>172</v>
       </c>
@@ -9847,8 +9679,8 @@
         <f>IF(AND(ISNUMBER(B40),ISNUMBER(C40)),MAX(A1:A39)+1,"")</f>
         <v/>
       </c>
-      <c r="B40" s="47"/>
-      <c r="C40" s="47"/>
+      <c r="B40" s="64"/>
+      <c r="C40" s="64"/>
       <c r="D40" s="15" t="s">
         <v>172</v>
       </c>
@@ -9858,8 +9690,8 @@
         <f>IF(AND(ISNUMBER(B41),ISNUMBER(C41)),MAX(A1:A40)+1,"")</f>
         <v/>
       </c>
-      <c r="B41" s="47"/>
-      <c r="C41" s="47"/>
+      <c r="B41" s="64"/>
+      <c r="C41" s="64"/>
       <c r="D41" s="15" t="s">
         <v>172</v>
       </c>
@@ -9869,8 +9701,8 @@
         <f>IF(AND(ISNUMBER(B42),ISNUMBER(C42)),MAX(A1:A41)+1,"")</f>
         <v/>
       </c>
-      <c r="B42" s="47"/>
-      <c r="C42" s="47"/>
+      <c r="B42" s="64"/>
+      <c r="C42" s="64"/>
       <c r="D42" s="15" t="s">
         <v>172</v>
       </c>
@@ -9880,8 +9712,8 @@
         <f>IF(AND(ISNUMBER(B43),ISNUMBER(C43)),MAX(A1:A42)+1,"")</f>
         <v/>
       </c>
-      <c r="B43" s="47"/>
-      <c r="C43" s="47"/>
+      <c r="B43" s="64"/>
+      <c r="C43" s="64"/>
       <c r="D43" s="15" t="s">
         <v>172</v>
       </c>
@@ -9891,8 +9723,8 @@
         <f>IF(AND(ISNUMBER(B44),ISNUMBER(C44)),MAX(A1:A43)+1,"")</f>
         <v/>
       </c>
-      <c r="B44" s="47"/>
-      <c r="C44" s="47"/>
+      <c r="B44" s="64"/>
+      <c r="C44" s="64"/>
       <c r="D44" s="15" t="s">
         <v>172</v>
       </c>
@@ -9902,8 +9734,8 @@
         <f>IF(AND(ISNUMBER(B45),ISNUMBER(C45)),MAX(A1:A44)+1,"")</f>
         <v/>
       </c>
-      <c r="B45" s="47"/>
-      <c r="C45" s="47"/>
+      <c r="B45" s="64"/>
+      <c r="C45" s="64"/>
       <c r="D45" s="15" t="s">
         <v>172</v>
       </c>
@@ -9913,8 +9745,8 @@
         <f>IF(AND(ISNUMBER(B46),ISNUMBER(C46)),MAX(A1:A45)+1,"")</f>
         <v/>
       </c>
-      <c r="B46" s="47"/>
-      <c r="C46" s="47"/>
+      <c r="B46" s="64"/>
+      <c r="C46" s="64"/>
       <c r="D46" s="15" t="s">
         <v>172</v>
       </c>
@@ -9924,8 +9756,8 @@
         <f>IF(AND(ISNUMBER(B47),ISNUMBER(C47)),MAX(A1:A46)+1,"")</f>
         <v/>
       </c>
-      <c r="B47" s="47"/>
-      <c r="C47" s="47"/>
+      <c r="B47" s="64"/>
+      <c r="C47" s="64"/>
       <c r="D47" s="15" t="s">
         <v>172</v>
       </c>
@@ -9935,8 +9767,8 @@
         <f>IF(AND(ISNUMBER(B48),ISNUMBER(C48)),MAX(A1:A47)+1,"")</f>
         <v/>
       </c>
-      <c r="B48" s="47"/>
-      <c r="C48" s="47"/>
+      <c r="B48" s="64"/>
+      <c r="C48" s="64"/>
       <c r="D48" s="15" t="s">
         <v>172</v>
       </c>
@@ -9946,8 +9778,8 @@
         <f>IF(AND(ISNUMBER(B49),ISNUMBER(C49)),MAX(A1:A48)+1,"")</f>
         <v/>
       </c>
-      <c r="B49" s="47"/>
-      <c r="C49" s="47"/>
+      <c r="B49" s="64"/>
+      <c r="C49" s="64"/>
       <c r="D49" s="15" t="s">
         <v>172</v>
       </c>
@@ -9957,8 +9789,8 @@
         <f>IF(AND(ISNUMBER(B50),ISNUMBER(C50)),MAX(A1:A49)+1,"")</f>
         <v/>
       </c>
-      <c r="B50" s="47"/>
-      <c r="C50" s="47"/>
+      <c r="B50" s="64"/>
+      <c r="C50" s="64"/>
       <c r="D50" s="15" t="s">
         <v>172</v>
       </c>
@@ -9968,8 +9800,8 @@
         <f>IF(AND(ISNUMBER(B51),ISNUMBER(C51)),MAX(A1:A50)+1,"")</f>
         <v/>
       </c>
-      <c r="B51" s="47"/>
-      <c r="C51" s="47"/>
+      <c r="B51" s="64"/>
+      <c r="C51" s="64"/>
       <c r="D51" s="15" t="s">
         <v>172</v>
       </c>
@@ -9979,8 +9811,8 @@
         <f>IF(AND(ISNUMBER(B52),ISNUMBER(C52)),MAX(A1:A51)+1,"")</f>
         <v/>
       </c>
-      <c r="B52" s="47"/>
-      <c r="C52" s="47"/>
+      <c r="B52" s="64"/>
+      <c r="C52" s="64"/>
       <c r="D52" s="15" t="s">
         <v>172</v>
       </c>
@@ -9990,8 +9822,8 @@
         <f>IF(AND(ISNUMBER(B53),ISNUMBER(C53)),MAX(A1:A52)+1,"")</f>
         <v/>
       </c>
-      <c r="B53" s="47"/>
-      <c r="C53" s="47"/>
+      <c r="B53" s="64"/>
+      <c r="C53" s="64"/>
       <c r="D53" s="15" t="s">
         <v>172</v>
       </c>
@@ -10001,8 +9833,8 @@
         <f>IF(AND(ISNUMBER(B54),ISNUMBER(C54)),MAX(A1:A53)+1,"")</f>
         <v/>
       </c>
-      <c r="B54" s="47"/>
-      <c r="C54" s="47"/>
+      <c r="B54" s="64"/>
+      <c r="C54" s="64"/>
       <c r="D54" s="15" t="s">
         <v>172</v>
       </c>
@@ -10012,8 +9844,8 @@
         <f>IF(AND(ISNUMBER(B55),ISNUMBER(C55)),MAX(A1:A54)+1,"")</f>
         <v/>
       </c>
-      <c r="B55" s="47"/>
-      <c r="C55" s="47"/>
+      <c r="B55" s="64"/>
+      <c r="C55" s="64"/>
       <c r="D55" s="15" t="s">
         <v>172</v>
       </c>
@@ -10023,8 +9855,8 @@
         <f>IF(AND(ISNUMBER(B56),ISNUMBER(C56)),MAX(A1:A55)+1,"")</f>
         <v/>
       </c>
-      <c r="B56" s="47"/>
-      <c r="C56" s="47"/>
+      <c r="B56" s="64"/>
+      <c r="C56" s="64"/>
       <c r="D56" s="15" t="s">
         <v>172</v>
       </c>
@@ -10034,8 +9866,8 @@
         <f>IF(AND(ISNUMBER(B57),ISNUMBER(C57)),MAX(A1:A56)+1,"")</f>
         <v/>
       </c>
-      <c r="B57" s="47"/>
-      <c r="C57" s="47"/>
+      <c r="B57" s="64"/>
+      <c r="C57" s="64"/>
       <c r="D57" s="15" t="s">
         <v>172</v>
       </c>
@@ -10045,8 +9877,8 @@
         <f>IF(AND(ISNUMBER(B58),ISNUMBER(C58)),MAX(A1:A57)+1,"")</f>
         <v/>
       </c>
-      <c r="B58" s="47"/>
-      <c r="C58" s="47"/>
+      <c r="B58" s="64"/>
+      <c r="C58" s="64"/>
       <c r="D58" s="15" t="s">
         <v>172</v>
       </c>
@@ -10056,8 +9888,8 @@
         <f>IF(AND(ISNUMBER(B59),ISNUMBER(C59)),MAX(A1:A58)+1,"")</f>
         <v/>
       </c>
-      <c r="B59" s="47"/>
-      <c r="C59" s="47"/>
+      <c r="B59" s="64"/>
+      <c r="C59" s="64"/>
       <c r="D59" s="15" t="s">
         <v>172</v>
       </c>
@@ -10067,8 +9899,8 @@
         <f>IF(AND(ISNUMBER(B60),ISNUMBER(C60)),MAX(A1:A59)+1,"")</f>
         <v/>
       </c>
-      <c r="B60" s="47"/>
-      <c r="C60" s="47"/>
+      <c r="B60" s="64"/>
+      <c r="C60" s="64"/>
       <c r="D60" s="15" t="s">
         <v>172</v>
       </c>
@@ -10078,8 +9910,8 @@
         <f>IF(AND(ISNUMBER(B61),ISNUMBER(C61)),MAX(A1:A60)+1,"")</f>
         <v/>
       </c>
-      <c r="B61" s="47"/>
-      <c r="C61" s="47"/>
+      <c r="B61" s="64"/>
+      <c r="C61" s="64"/>
       <c r="D61" s="15" t="s">
         <v>172</v>
       </c>
@@ -10089,8 +9921,8 @@
         <f>IF(AND(ISNUMBER(B62),ISNUMBER(C62)),MAX(A1:A61)+1,"")</f>
         <v/>
       </c>
-      <c r="B62" s="47"/>
-      <c r="C62" s="47"/>
+      <c r="B62" s="64"/>
+      <c r="C62" s="64"/>
       <c r="D62" s="15" t="s">
         <v>172</v>
       </c>
@@ -10100,8 +9932,8 @@
         <f>IF(AND(ISNUMBER(B63),ISNUMBER(C63)),MAX(A1:A62)+1,"")</f>
         <v/>
       </c>
-      <c r="B63" s="47"/>
-      <c r="C63" s="47"/>
+      <c r="B63" s="64"/>
+      <c r="C63" s="64"/>
       <c r="D63" s="15" t="s">
         <v>172</v>
       </c>
@@ -10111,8 +9943,8 @@
         <f>IF(AND(ISNUMBER(B64),ISNUMBER(C64)),MAX(A1:A63)+1,"")</f>
         <v/>
       </c>
-      <c r="B64" s="47"/>
-      <c r="C64" s="47"/>
+      <c r="B64" s="64"/>
+      <c r="C64" s="64"/>
       <c r="D64" s="15" t="s">
         <v>172</v>
       </c>
@@ -10122,8 +9954,8 @@
         <f>IF(AND(ISNUMBER(B65),ISNUMBER(C65)),MAX(A1:A64)+1,"")</f>
         <v/>
       </c>
-      <c r="B65" s="47"/>
-      <c r="C65" s="47"/>
+      <c r="B65" s="64"/>
+      <c r="C65" s="64"/>
       <c r="D65" s="15" t="s">
         <v>172</v>
       </c>
@@ -10133,8 +9965,8 @@
         <f>IF(AND(ISNUMBER(B66),ISNUMBER(C66)),MAX(A1:A65)+1,"")</f>
         <v/>
       </c>
-      <c r="B66" s="47"/>
-      <c r="C66" s="47"/>
+      <c r="B66" s="64"/>
+      <c r="C66" s="64"/>
       <c r="D66" s="15" t="s">
         <v>172</v>
       </c>
@@ -10144,8 +9976,8 @@
         <f>IF(AND(ISNUMBER(B67),ISNUMBER(C67)),MAX(A1:A66)+1,"")</f>
         <v/>
       </c>
-      <c r="B67" s="47"/>
-      <c r="C67" s="47"/>
+      <c r="B67" s="64"/>
+      <c r="C67" s="64"/>
       <c r="D67" s="15" t="s">
         <v>172</v>
       </c>
@@ -10155,8 +9987,8 @@
         <f>IF(AND(ISNUMBER(B68),ISNUMBER(C68)),MAX(A1:A67)+1,"")</f>
         <v/>
       </c>
-      <c r="B68" s="47"/>
-      <c r="C68" s="47"/>
+      <c r="B68" s="64"/>
+      <c r="C68" s="64"/>
       <c r="D68" s="15" t="s">
         <v>172</v>
       </c>
@@ -10166,8 +9998,8 @@
         <f>IF(AND(ISNUMBER(B69),ISNUMBER(C69)),MAX(A1:A68)+1,"")</f>
         <v/>
       </c>
-      <c r="B69" s="47"/>
-      <c r="C69" s="47"/>
+      <c r="B69" s="64"/>
+      <c r="C69" s="64"/>
       <c r="D69" s="15" t="s">
         <v>172</v>
       </c>
@@ -10177,8 +10009,8 @@
         <f>IF(AND(ISNUMBER(B70),ISNUMBER(C70)),MAX(A1:A69)+1,"")</f>
         <v/>
       </c>
-      <c r="B70" s="47"/>
-      <c r="C70" s="47"/>
+      <c r="B70" s="64"/>
+      <c r="C70" s="64"/>
       <c r="D70" s="15" t="s">
         <v>172</v>
       </c>
@@ -10188,8 +10020,8 @@
         <f>IF(AND(ISNUMBER(B71),ISNUMBER(C71)),MAX(A1:A70)+1,"")</f>
         <v/>
       </c>
-      <c r="B71" s="47"/>
-      <c r="C71" s="47"/>
+      <c r="B71" s="64"/>
+      <c r="C71" s="64"/>
       <c r="D71" s="15" t="s">
         <v>172</v>
       </c>
@@ -10199,8 +10031,8 @@
         <f>IF(AND(ISNUMBER(B72),ISNUMBER(C72)),MAX(A1:A71)+1,"")</f>
         <v/>
       </c>
-      <c r="B72" s="47"/>
-      <c r="C72" s="47"/>
+      <c r="B72" s="64"/>
+      <c r="C72" s="64"/>
       <c r="D72" s="15" t="s">
         <v>172</v>
       </c>
@@ -10210,8 +10042,8 @@
         <f>IF(AND(ISNUMBER(B73),ISNUMBER(C73)),MAX(A1:A72)+1,"")</f>
         <v/>
       </c>
-      <c r="B73" s="47"/>
-      <c r="C73" s="47"/>
+      <c r="B73" s="64"/>
+      <c r="C73" s="64"/>
       <c r="D73" s="15" t="s">
         <v>172</v>
       </c>
@@ -10221,8 +10053,8 @@
         <f>IF(AND(ISNUMBER(B74),ISNUMBER(C74)),MAX(A1:A73)+1,"")</f>
         <v/>
       </c>
-      <c r="B74" s="47"/>
-      <c r="C74" s="47"/>
+      <c r="B74" s="64"/>
+      <c r="C74" s="64"/>
       <c r="D74" s="15" t="s">
         <v>172</v>
       </c>
@@ -10232,8 +10064,8 @@
         <f>IF(AND(ISNUMBER(B75),ISNUMBER(C75)),MAX(A1:A74)+1,"")</f>
         <v/>
       </c>
-      <c r="B75" s="47"/>
-      <c r="C75" s="47"/>
+      <c r="B75" s="64"/>
+      <c r="C75" s="64"/>
       <c r="D75" s="15" t="s">
         <v>172</v>
       </c>
@@ -10243,8 +10075,8 @@
         <f>IF(AND(ISNUMBER(B76),ISNUMBER(C76)),MAX(A1:A75)+1,"")</f>
         <v/>
       </c>
-      <c r="B76" s="47"/>
-      <c r="C76" s="47"/>
+      <c r="B76" s="64"/>
+      <c r="C76" s="64"/>
       <c r="D76" s="15" t="s">
         <v>172</v>
       </c>
@@ -10254,8 +10086,8 @@
         <f>IF(AND(ISNUMBER(B77),ISNUMBER(C77)),MAX(A1:A76)+1,"")</f>
         <v/>
       </c>
-      <c r="B77" s="47"/>
-      <c r="C77" s="47"/>
+      <c r="B77" s="64"/>
+      <c r="C77" s="64"/>
       <c r="D77" s="15" t="s">
         <v>172</v>
       </c>
@@ -10265,8 +10097,8 @@
         <f>IF(AND(ISNUMBER(B78),ISNUMBER(C78)),MAX(A1:A77)+1,"")</f>
         <v/>
       </c>
-      <c r="B78" s="47"/>
-      <c r="C78" s="47"/>
+      <c r="B78" s="64"/>
+      <c r="C78" s="64"/>
       <c r="D78" s="15" t="s">
         <v>172</v>
       </c>
@@ -10276,8 +10108,8 @@
         <f>IF(AND(ISNUMBER(B79),ISNUMBER(C79)),MAX(A1:A78)+1,"")</f>
         <v/>
       </c>
-      <c r="B79" s="47"/>
-      <c r="C79" s="47"/>
+      <c r="B79" s="64"/>
+      <c r="C79" s="64"/>
       <c r="D79" s="15" t="s">
         <v>172</v>
       </c>
@@ -10287,8 +10119,8 @@
         <f>IF(AND(ISNUMBER(B80),ISNUMBER(C80)),MAX(A1:A79)+1,"")</f>
         <v/>
       </c>
-      <c r="B80" s="47"/>
-      <c r="C80" s="47"/>
+      <c r="B80" s="64"/>
+      <c r="C80" s="64"/>
       <c r="D80" s="15" t="s">
         <v>172</v>
       </c>
@@ -10298,8 +10130,8 @@
         <f>IF(AND(ISNUMBER(B81),ISNUMBER(C81)),MAX(A1:A80)+1,"")</f>
         <v/>
       </c>
-      <c r="B81" s="47"/>
-      <c r="C81" s="47"/>
+      <c r="B81" s="64"/>
+      <c r="C81" s="64"/>
       <c r="D81" s="15" t="s">
         <v>172</v>
       </c>
@@ -10309,8 +10141,8 @@
         <f>IF(AND(ISNUMBER(B82),ISNUMBER(C82)),MAX(A1:A81)+1,"")</f>
         <v/>
       </c>
-      <c r="B82" s="47"/>
-      <c r="C82" s="47"/>
+      <c r="B82" s="64"/>
+      <c r="C82" s="64"/>
       <c r="D82" s="15" t="s">
         <v>172</v>
       </c>
@@ -10320,8 +10152,8 @@
         <f>IF(AND(ISNUMBER(B83),ISNUMBER(C83)),MAX(A1:A82)+1,"")</f>
         <v/>
       </c>
-      <c r="B83" s="47"/>
-      <c r="C83" s="47"/>
+      <c r="B83" s="64"/>
+      <c r="C83" s="64"/>
       <c r="D83" s="15" t="s">
         <v>172</v>
       </c>
@@ -10331,8 +10163,8 @@
         <f>IF(AND(ISNUMBER(B84),ISNUMBER(C84)),MAX(A1:A83)+1,"")</f>
         <v/>
       </c>
-      <c r="B84" s="47"/>
-      <c r="C84" s="47"/>
+      <c r="B84" s="64"/>
+      <c r="C84" s="64"/>
       <c r="D84" s="15" t="s">
         <v>172</v>
       </c>
@@ -10342,8 +10174,8 @@
         <f>IF(AND(ISNUMBER(B85),ISNUMBER(C85)),MAX(A1:A84)+1,"")</f>
         <v/>
       </c>
-      <c r="B85" s="47"/>
-      <c r="C85" s="47"/>
+      <c r="B85" s="64"/>
+      <c r="C85" s="64"/>
       <c r="D85" s="15" t="s">
         <v>172</v>
       </c>
@@ -10353,8 +10185,8 @@
         <f>IF(AND(ISNUMBER(B86),ISNUMBER(C86)),MAX(A1:A85)+1,"")</f>
         <v/>
       </c>
-      <c r="B86" s="47"/>
-      <c r="C86" s="47"/>
+      <c r="B86" s="64"/>
+      <c r="C86" s="64"/>
       <c r="D86" s="15" t="s">
         <v>172</v>
       </c>
@@ -10364,8 +10196,8 @@
         <f>IF(AND(ISNUMBER(B87),ISNUMBER(C87)),MAX(A1:A86)+1,"")</f>
         <v/>
       </c>
-      <c r="B87" s="47"/>
-      <c r="C87" s="47"/>
+      <c r="B87" s="64"/>
+      <c r="C87" s="64"/>
       <c r="D87" s="15" t="s">
         <v>172</v>
       </c>
@@ -10375,8 +10207,8 @@
         <f>IF(AND(ISNUMBER(B88),ISNUMBER(C88)),MAX(A1:A87)+1,"")</f>
         <v/>
       </c>
-      <c r="B88" s="47"/>
-      <c r="C88" s="47"/>
+      <c r="B88" s="64"/>
+      <c r="C88" s="64"/>
       <c r="D88" s="15" t="s">
         <v>172</v>
       </c>
@@ -10386,8 +10218,8 @@
         <f>IF(AND(ISNUMBER(B89),ISNUMBER(C89)),MAX(A1:A88)+1,"")</f>
         <v/>
       </c>
-      <c r="B89" s="47"/>
-      <c r="C89" s="47"/>
+      <c r="B89" s="64"/>
+      <c r="C89" s="64"/>
       <c r="D89" s="15" t="s">
         <v>172</v>
       </c>
@@ -10397,8 +10229,8 @@
         <f>IF(AND(ISNUMBER(B90),ISNUMBER(C90)),MAX(A1:A89)+1,"")</f>
         <v/>
       </c>
-      <c r="B90" s="47"/>
-      <c r="C90" s="47"/>
+      <c r="B90" s="64"/>
+      <c r="C90" s="64"/>
       <c r="D90" s="15" t="s">
         <v>172</v>
       </c>
@@ -10408,8 +10240,8 @@
         <f>IF(AND(ISNUMBER(B91),ISNUMBER(C91)),MAX(A1:A90)+1,"")</f>
         <v/>
       </c>
-      <c r="B91" s="47"/>
-      <c r="C91" s="47"/>
+      <c r="B91" s="64"/>
+      <c r="C91" s="64"/>
       <c r="D91" s="15" t="s">
         <v>172</v>
       </c>
@@ -10419,8 +10251,8 @@
         <f>IF(AND(ISNUMBER(B92),ISNUMBER(C92)),MAX(A1:A91)+1,"")</f>
         <v/>
       </c>
-      <c r="B92" s="47"/>
-      <c r="C92" s="47"/>
+      <c r="B92" s="64"/>
+      <c r="C92" s="64"/>
       <c r="D92" s="15" t="s">
         <v>172</v>
       </c>
@@ -10430,8 +10262,8 @@
         <f>IF(AND(ISNUMBER(B93),ISNUMBER(C93)),MAX(A1:A92)+1,"")</f>
         <v/>
       </c>
-      <c r="B93" s="47"/>
-      <c r="C93" s="47"/>
+      <c r="B93" s="64"/>
+      <c r="C93" s="64"/>
       <c r="D93" s="15" t="s">
         <v>172</v>
       </c>
@@ -10441,8 +10273,8 @@
         <f>IF(AND(ISNUMBER(B94),ISNUMBER(C94)),MAX(A1:A93)+1,"")</f>
         <v/>
       </c>
-      <c r="B94" s="47"/>
-      <c r="C94" s="47"/>
+      <c r="B94" s="64"/>
+      <c r="C94" s="64"/>
       <c r="D94" s="15" t="s">
         <v>172</v>
       </c>
@@ -10452,8 +10284,8 @@
         <f>IF(AND(ISNUMBER(B95),ISNUMBER(C95)),MAX(A1:A94)+1,"")</f>
         <v/>
       </c>
-      <c r="B95" s="47"/>
-      <c r="C95" s="47"/>
+      <c r="B95" s="64"/>
+      <c r="C95" s="64"/>
       <c r="D95" s="15" t="s">
         <v>172</v>
       </c>
@@ -10463,8 +10295,8 @@
         <f>IF(AND(ISNUMBER(B96),ISNUMBER(C96)),MAX(A1:A95)+1,"")</f>
         <v/>
       </c>
-      <c r="B96" s="47"/>
-      <c r="C96" s="47"/>
+      <c r="B96" s="64"/>
+      <c r="C96" s="64"/>
       <c r="D96" s="15" t="s">
         <v>172</v>
       </c>
@@ -10474,8 +10306,8 @@
         <f>IF(AND(ISNUMBER(B97),ISNUMBER(C97)),MAX(A1:A96)+1,"")</f>
         <v/>
       </c>
-      <c r="B97" s="47"/>
-      <c r="C97" s="47"/>
+      <c r="B97" s="64"/>
+      <c r="C97" s="64"/>
       <c r="D97" s="15" t="s">
         <v>172</v>
       </c>
@@ -10485,8 +10317,8 @@
         <f>IF(AND(ISNUMBER(B98),ISNUMBER(C98)),MAX(A1:A97)+1,"")</f>
         <v/>
       </c>
-      <c r="B98" s="47"/>
-      <c r="C98" s="47"/>
+      <c r="B98" s="64"/>
+      <c r="C98" s="64"/>
       <c r="D98" s="15" t="s">
         <v>172</v>
       </c>
@@ -10496,8 +10328,8 @@
         <f>IF(AND(ISNUMBER(B99),ISNUMBER(C99)),MAX(A1:A98)+1,"")</f>
         <v/>
       </c>
-      <c r="B99" s="47"/>
-      <c r="C99" s="47"/>
+      <c r="B99" s="64"/>
+      <c r="C99" s="64"/>
       <c r="D99" s="15" t="s">
         <v>172</v>
       </c>
@@ -10507,8 +10339,8 @@
         <f>IF(AND(ISNUMBER(B100),ISNUMBER(C100)),MAX(A1:A99)+1,"")</f>
         <v/>
       </c>
-      <c r="B100" s="47"/>
-      <c r="C100" s="47"/>
+      <c r="B100" s="64"/>
+      <c r="C100" s="64"/>
       <c r="D100" s="15" t="s">
         <v>172</v>
       </c>
@@ -10518,8 +10350,8 @@
         <f>IF(AND(ISNUMBER(B101),ISNUMBER(C101)),MAX(A1:A100)+1,"")</f>
         <v/>
       </c>
-      <c r="B101" s="47"/>
-      <c r="C101" s="47"/>
+      <c r="B101" s="64"/>
+      <c r="C101" s="64"/>
       <c r="D101" s="15" t="s">
         <v>172</v>
       </c>
@@ -10529,13 +10361,14 @@
         <f>IF(AND(ISNUMBER(B102),ISNUMBER(C102)),MAX(A1:A101)+1,"")</f>
         <v/>
       </c>
-      <c r="B102" s="47"/>
-      <c r="C102" s="47"/>
+      <c r="B102" s="64"/>
+      <c r="C102" s="64"/>
       <c r="D102" s="15" t="s">
         <v>172</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="R5ow5K8laFcG3RIGTRSp29rit17ANP7Z7sX7TIz6Tjyr9WOrmy04qldVIXqo1r0dbFzwyYf6KbvfNuKTTJeK+w==" saltValue="iBkDjQAC76x4MLWGCVKadQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" sort="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -10570,7 +10403,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="55" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="40"/>
@@ -10586,7 +10419,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="55" t="s">
         <v>51</v>
       </c>
       <c r="B3" s="40"/>
@@ -10598,12 +10431,12 @@
         <f>IF(AND(ISNUMBER(B2),ISNUMBER(B3),B3&gt;=0,B3&lt;=1,B2&gt;=0,B2&lt;=50),0," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E3" s="58" t="str">
+      <c r="E3" s="57" t="str">
         <f>IF(ISNUMBER(D3),COMBIN(B2,D3)*B3^D3*(1-B3)^(B2-D3),"")</f>
         <v/>
       </c>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
@@ -10612,12 +10445,12 @@
         <f>IF(AND(ISNUMBER(D3),D3&lt;B2),D3+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E4" s="58" t="str">
+      <c r="E4" s="57" t="str">
         <f>IF(ISNUMBER(D4),COMBIN(B2,D4)*B3^D4*(1-B3)^(B2-D4),"")</f>
         <v/>
       </c>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
@@ -10628,15 +10461,15 @@
         <f>IF(AND(ISNUMBER(D4),D4&lt;B2),D4+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E5" s="58" t="str">
+      <c r="E5" s="57" t="str">
         <f>IF(ISNUMBER(D5),COMBIN(B2,D5)*B3^D5*(1-B3)^(B2-D5),"")</f>
         <v/>
       </c>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="55" t="s">
         <v>53</v>
       </c>
       <c r="B6" s="40"/>
@@ -10648,18 +10481,18 @@
         <f>IF(AND(ISNUMBER(D5),D5&lt;B2),D5+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E6" s="58" t="str">
+      <c r="E6" s="57" t="str">
         <f>IF(ISNUMBER(D6),COMBIN(B2,D6)*B3^D6*(1-B3)^(B2-D6),"")</f>
         <v/>
       </c>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="57" t="str">
+      <c r="B7" s="56" t="str">
         <f>IF(ISNUMBER(B6),IF(AND(B2&gt;0,INT(B2)=B2,NOT(ISBLANK(B3)),B3&gt;=0,B3&lt;=1,B6&gt;=0,B6&lt;=B2,INT(B6)=B6),COMBIN(B2,B6)*B3^B6*(1-B3)^(B2-B6),"Input error"),"")</f>
         <v/>
       </c>
@@ -10670,12 +10503,12 @@
         <f>IF(AND(ISNUMBER(D6),D6&lt;B2),D6+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E7" s="58" t="str">
+      <c r="E7" s="57" t="str">
         <f>IF(ISNUMBER(D7),COMBIN(B2,D7)*B3^D7*(1-B3)^(B2-D7),"")</f>
         <v/>
       </c>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C8" s="12"/>
@@ -10683,12 +10516,12 @@
         <f>IF(AND(ISNUMBER(D7),D7&lt;B2),D7+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E8" s="58" t="str">
+      <c r="E8" s="57" t="str">
         <f>IF(ISNUMBER(D8),COMBIN(B2,D8)*B3^D8*(1-B3)^(B2-D8),"")</f>
         <v/>
       </c>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
@@ -10699,15 +10532,15 @@
         <f>IF(AND(ISNUMBER(D8),D8&lt;B2),D8+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E9" s="58" t="str">
+      <c r="E9" s="57" t="str">
         <f>IF(ISNUMBER(D9),COMBIN(B2,D9)*B3^D9*(1-B3)^(B2-D9),"")</f>
         <v/>
       </c>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="55" t="s">
         <v>57</v>
       </c>
       <c r="B10" s="40"/>
@@ -10718,15 +10551,15 @@
         <f>IF(AND(ISNUMBER(D9),D9&lt;B2),D9+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E10" s="58" t="str">
+      <c r="E10" s="57" t="str">
         <f>IF(ISNUMBER(D10),COMBIN(B2,D10)*B3^D10*(1-B3)^(B2-D10),"")</f>
         <v/>
       </c>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="55" t="s">
         <v>59</v>
       </c>
       <c r="B11" s="40"/>
@@ -10737,19 +10570,19 @@
         <f>IF(AND(ISNUMBER(D10),D10&lt;B2),D10+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E11" s="58" t="str">
+      <c r="E11" s="57" t="str">
         <f>IF(ISNUMBER(D11),COMBIN(B2,D11)*B3^D11*(1-B3)^(B2-D11),"")</f>
         <v/>
       </c>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="56" t="str">
+      <c r="A12" s="55" t="str">
         <f>CONCATENATE("P(", IF(ISBLANK(B10),"","lower ≤ "),"x",IF(ISBLANK(B11),""," ≤ upper"),") =")</f>
         <v>P(x) =</v>
       </c>
-      <c r="B12" s="57" t="str">
+      <c r="B12" s="56" t="str">
         <f>IF(OR(ISNUMBER(B10),ISNUMBER(B11)),IF(AND(B2&gt;0,B2&lt;=50,INT(B2)=B2,NOT(ISBLANK(B3)),B3&gt;=0,B3&lt;=1, OR(ISBLANK(B10),AND(B10&gt;=0,B10&lt;=B2,IF(ISNUMBER(B10),INT(B10)=B10,FALSE),OR(ISBLANK(B11),B10&lt;=B11))),OR(ISBLANK(B11),AND(B11&gt;=0,B11&lt;=B2,IF(ISNUMBER(B11),INT(B11)=B11,FALSE),OR(ISBLANK(B10),B10&lt;=B11)))),IF(ISBLANK(B10),SUMIF(D3:D53,"&lt;="&amp;B11,E3:E53),IF(ISBLANK(B11),SUMIF(D3:D53,"&gt;="&amp;B10,E3:E53),SUMIF(D3:D53,"&lt;="&amp;B11,E3:E53)-SUMIF(D3:D53,"&lt;"&amp;B10,E3:E53))),"Input error"),"")</f>
         <v/>
       </c>
@@ -10760,509 +10593,509 @@
         <f>IF(AND(ISNUMBER(D11),D11&lt;B2),D11+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E12" s="58" t="str">
+      <c r="E12" s="57" t="str">
         <f>IF(ISNUMBER(D12),COMBIN(B2,D12)*B3^D12*(1-B3)^(B2-D12),"")</f>
         <v/>
       </c>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="50" t="str">
+      <c r="A13" s="49" t="str">
         <f>IF(AND(NOT(AND(ISBLANK(B10),ISBLANK(B11))),B2&gt;50),"Binomial Range tool in Respondus currently only works for n &lt;= 50"," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="B13" s="51"/>
+      <c r="B13" s="50"/>
       <c r="D13" s="1" t="str">
         <f>IF(AND(ISNUMBER(D12),D12&lt;B2),D12+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E13" s="58" t="str">
+      <c r="E13" s="57" t="str">
         <f>IF(ISNUMBER(D13),COMBIN(B2,D13)*B3^D13*(1-B3)^(B2-D13),"")</f>
         <v/>
       </c>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="str">
         <f>IF(AND(ISNUMBER(D13),D13&lt;B2),D13+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E14" s="58" t="str">
+      <c r="E14" s="57" t="str">
         <f>IF(ISNUMBER(D14),COMBIN(B2,D14)*B3^D14*(1-B3)^(B2-D14),"")</f>
         <v/>
       </c>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="str">
         <f>IF(AND(ISNUMBER(D14),D14&lt;B2),D14+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E15" s="58" t="str">
+      <c r="E15" s="57" t="str">
         <f>IF(ISNUMBER(D15),COMBIN(B2,D15)*B3^D15*(1-B3)^(B2-D15),"")</f>
         <v/>
       </c>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="str">
         <f>IF(AND(ISNUMBER(D15),D15&lt;B2),D15+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E16" s="58" t="str">
+      <c r="E16" s="57" t="str">
         <f>IF(ISNUMBER(D16),COMBIN(B2,D16)*B3^D16*(1-B3)^(B2-D16),"")</f>
         <v/>
       </c>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D17" s="1" t="str">
         <f>IF(AND(ISNUMBER(D16),D16&lt;B2),D16+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E17" s="58" t="str">
+      <c r="E17" s="57" t="str">
         <f>IF(ISNUMBER(D17),COMBIN(B2,D17)*B3^D17*(1-B3)^(B2-D17),"")</f>
         <v/>
       </c>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D18" s="1" t="str">
         <f>IF(AND(ISNUMBER(D17),D17&lt;B2),D17+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E18" s="58" t="str">
+      <c r="E18" s="57" t="str">
         <f>IF(ISNUMBER(D18),COMBIN(B2,D18)*B3^D18*(1-B3)^(B2-D18),"")</f>
         <v/>
       </c>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D19" s="1" t="str">
         <f>IF(AND(ISNUMBER(D18),D18&lt;B2),D18+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E19" s="58" t="str">
+      <c r="E19" s="57" t="str">
         <f>IF(ISNUMBER(D19),COMBIN(B2,D19)*B3^D19*(1-B3)^(B2-D19),"")</f>
         <v/>
       </c>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D20" s="1" t="str">
         <f>IF(AND(ISNUMBER(D19),D19&lt;B2),D19+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E20" s="58" t="str">
+      <c r="E20" s="57" t="str">
         <f>IF(ISNUMBER(D20),COMBIN(B2,D20)*B3^D20*(1-B3)^(B2-D20),"")</f>
         <v/>
       </c>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D21" s="1" t="str">
         <f>IF(AND(ISNUMBER(D20),D20&lt;B2),D20+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E21" s="58" t="str">
+      <c r="E21" s="57" t="str">
         <f>IF(ISNUMBER(D21),COMBIN(B2,D21)*B3^D21*(1-B3)^(B2-D21),"")</f>
         <v/>
       </c>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
     </row>
     <row r="22" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D22" s="1" t="str">
         <f>IF(AND(ISNUMBER(D21),D21&lt;B2),D21+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E22" s="58" t="str">
+      <c r="E22" s="57" t="str">
         <f>IF(ISNUMBER(D22),COMBIN(B2,D22)*B3^D22*(1-B3)^(B2-D22),"")</f>
         <v/>
       </c>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
     </row>
     <row r="23" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D23" s="1" t="str">
         <f>IF(AND(ISNUMBER(D22),D22&lt;B2),D22+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E23" s="58" t="str">
+      <c r="E23" s="57" t="str">
         <f>IF(ISNUMBER(D23),COMBIN(B2,D23)*B3^D23*(1-B3)^(B2-D23),"")</f>
         <v/>
       </c>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
     </row>
     <row r="24" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D24" s="1" t="str">
         <f>IF(AND(ISNUMBER(D23),D23&lt;B2),D23+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E24" s="58" t="str">
+      <c r="E24" s="57" t="str">
         <f>IF(ISNUMBER(D24),COMBIN(B2,D24)*B3^D24*(1-B3)^(B2-D24),"")</f>
         <v/>
       </c>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
     </row>
     <row r="25" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D25" s="1" t="str">
         <f>IF(AND(ISNUMBER(D24),D24&lt;B2),D24+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E25" s="58" t="str">
+      <c r="E25" s="57" t="str">
         <f>IF(ISNUMBER(D25),COMBIN(B2,D25)*B3^D25*(1-B3)^(B2-D25),"")</f>
         <v/>
       </c>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D26" s="1" t="str">
         <f>IF(AND(ISNUMBER(D25),D25&lt;B2),D25+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E26" s="58" t="str">
+      <c r="E26" s="57" t="str">
         <f>IF(ISNUMBER(D26),COMBIN(B2,D26)*B3^D26*(1-B3)^(B2-D26),"")</f>
         <v/>
       </c>
-      <c r="F26" s="49"/>
-      <c r="G26" s="49"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="48"/>
     </row>
     <row r="27" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D27" s="1" t="str">
         <f>IF(AND(ISNUMBER(D26),D26&lt;B2),D26+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E27" s="58" t="str">
+      <c r="E27" s="57" t="str">
         <f>IF(ISNUMBER(D27),COMBIN(B2,D27)*B3^D27*(1-B3)^(B2-D27),"")</f>
         <v/>
       </c>
-      <c r="F27" s="49"/>
-      <c r="G27" s="49"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
     </row>
     <row r="28" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D28" s="1" t="str">
         <f>IF(AND(ISNUMBER(D27),D27&lt;B2),D27+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E28" s="58" t="str">
+      <c r="E28" s="57" t="str">
         <f>IF(ISNUMBER(D28),COMBIN(B2,D28)*B3^D28*(1-B3)^(B2-D28),"")</f>
         <v/>
       </c>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
     </row>
     <row r="29" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D29" s="1" t="str">
         <f>IF(AND(ISNUMBER(D28),D28&lt;B2),D28+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E29" s="58" t="str">
+      <c r="E29" s="57" t="str">
         <f>IF(ISNUMBER(D29),COMBIN(B2,D29)*B3^D29*(1-B3)^(B2-D29),"")</f>
         <v/>
       </c>
-      <c r="F29" s="49"/>
-      <c r="G29" s="49"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="48"/>
     </row>
     <row r="30" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D30" s="1" t="str">
         <f>IF(AND(ISNUMBER(D29),D29&lt;B2),D29+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E30" s="58" t="str">
+      <c r="E30" s="57" t="str">
         <f>IF(ISNUMBER(D30),COMBIN(B2,D30)*B3^D30*(1-B3)^(B2-D30),"")</f>
         <v/>
       </c>
-      <c r="F30" s="49"/>
-      <c r="G30" s="49"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="48"/>
     </row>
     <row r="31" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D31" s="1" t="str">
         <f>IF(AND(ISNUMBER(D30),D30&lt;B2),D30+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E31" s="58" t="str">
+      <c r="E31" s="57" t="str">
         <f>IF(ISNUMBER(D31),COMBIN(B2,D31)*B3^D31*(1-B3)^(B2-D31),"")</f>
         <v/>
       </c>
-      <c r="F31" s="49"/>
-      <c r="G31" s="49"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
     </row>
     <row r="32" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D32" s="1" t="str">
         <f>IF(AND(ISNUMBER(D31),D31&lt;B2),D31+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E32" s="58" t="str">
+      <c r="E32" s="57" t="str">
         <f>IF(ISNUMBER(D32),COMBIN(B2,D32)*B3^D32*(1-B3)^(B2-D32),"")</f>
         <v/>
       </c>
-      <c r="F32" s="49"/>
-      <c r="G32" s="49"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="48"/>
     </row>
     <row r="33" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D33" s="1" t="str">
         <f>IF(AND(ISNUMBER(D32),D32&lt;B2),D32+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E33" s="58" t="str">
+      <c r="E33" s="57" t="str">
         <f>IF(ISNUMBER(D33),COMBIN(B2,D33)*B3^D33*(1-B3)^(B2-D33),"")</f>
         <v/>
       </c>
-      <c r="F33" s="49"/>
-      <c r="G33" s="49"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="48"/>
     </row>
     <row r="34" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D34" s="1" t="str">
         <f>IF(AND(ISNUMBER(D33),D33&lt;B2),D33+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E34" s="58" t="str">
+      <c r="E34" s="57" t="str">
         <f>IF(ISNUMBER(D34),COMBIN(B2,D34)*B3^D34*(1-B3)^(B2-D34),"")</f>
         <v/>
       </c>
-      <c r="F34" s="49"/>
-      <c r="G34" s="49"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="48"/>
     </row>
     <row r="35" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D35" s="1" t="str">
         <f>IF(AND(ISNUMBER(D34),D34&lt;B2),D34+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E35" s="58" t="str">
+      <c r="E35" s="57" t="str">
         <f>IF(ISNUMBER(D35),COMBIN(B2,D35)*B3^D35*(1-B3)^(B2-D35),"")</f>
         <v/>
       </c>
-      <c r="F35" s="49"/>
-      <c r="G35" s="49"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="48"/>
     </row>
     <row r="36" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D36" s="1" t="str">
         <f>IF(AND(ISNUMBER(D35),D35&lt;B2),D35+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E36" s="58" t="str">
+      <c r="E36" s="57" t="str">
         <f>IF(ISNUMBER(D36),COMBIN(B2,D36)*B3^D36*(1-B3)^(B2-D36),"")</f>
         <v/>
       </c>
-      <c r="F36" s="49"/>
-      <c r="G36" s="49"/>
+      <c r="F36" s="48"/>
+      <c r="G36" s="48"/>
     </row>
     <row r="37" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D37" s="1" t="str">
         <f>IF(AND(ISNUMBER(D36),D36&lt;B2),D36+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E37" s="58" t="str">
+      <c r="E37" s="57" t="str">
         <f>IF(ISNUMBER(D37),COMBIN(B2,D37)*B3^D37*(1-B3)^(B2-D37),"")</f>
         <v/>
       </c>
-      <c r="F37" s="49"/>
-      <c r="G37" s="49"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="48"/>
     </row>
     <row r="38" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D38" s="1" t="str">
         <f>IF(AND(ISNUMBER(D37),D37&lt;B2),D37+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E38" s="58" t="str">
+      <c r="E38" s="57" t="str">
         <f>IF(ISNUMBER(D38),COMBIN(B2,D38)*B3^D38*(1-B3)^(B2-D38),"")</f>
         <v/>
       </c>
-      <c r="F38" s="49"/>
-      <c r="G38" s="49"/>
+      <c r="F38" s="48"/>
+      <c r="G38" s="48"/>
     </row>
     <row r="39" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D39" s="1" t="str">
         <f>IF(AND(ISNUMBER(D38),D38&lt;B2),D38+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E39" s="58" t="str">
+      <c r="E39" s="57" t="str">
         <f>IF(ISNUMBER(D39),COMBIN(B2,D39)*B3^D39*(1-B3)^(B2-D39),"")</f>
         <v/>
       </c>
-      <c r="F39" s="49"/>
-      <c r="G39" s="49"/>
+      <c r="F39" s="48"/>
+      <c r="G39" s="48"/>
     </row>
     <row r="40" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D40" s="1" t="str">
         <f>IF(AND(ISNUMBER(D39),D39&lt;B2),D39+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E40" s="58" t="str">
+      <c r="E40" s="57" t="str">
         <f>IF(ISNUMBER(D40),COMBIN(B2,D40)*B3^D40*(1-B3)^(B2-D40),"")</f>
         <v/>
       </c>
-      <c r="F40" s="49"/>
-      <c r="G40" s="49"/>
+      <c r="F40" s="48"/>
+      <c r="G40" s="48"/>
     </row>
     <row r="41" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D41" s="1" t="str">
         <f>IF(AND(ISNUMBER(D40),D40&lt;B2),D40+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E41" s="58" t="str">
+      <c r="E41" s="57" t="str">
         <f>IF(ISNUMBER(D41),COMBIN(B2,D41)*B3^D41*(1-B3)^(B2-D41),"")</f>
         <v/>
       </c>
-      <c r="F41" s="49"/>
-      <c r="G41" s="49"/>
+      <c r="F41" s="48"/>
+      <c r="G41" s="48"/>
     </row>
     <row r="42" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D42" s="1" t="str">
         <f>IF(AND(ISNUMBER(D41),D41&lt;B2),D41+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E42" s="58" t="str">
+      <c r="E42" s="57" t="str">
         <f>IF(ISNUMBER(D42),COMBIN(B2,D42)*B3^D42*(1-B3)^(B2-D42),"")</f>
         <v/>
       </c>
-      <c r="F42" s="49"/>
-      <c r="G42" s="49"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="48"/>
     </row>
     <row r="43" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D43" s="1" t="str">
         <f>IF(AND(ISNUMBER(D42),D42&lt;B2),D42+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E43" s="58" t="str">
+      <c r="E43" s="57" t="str">
         <f>IF(ISNUMBER(D43),COMBIN(B2,D43)*B3^D43*(1-B3)^(B2-D43),"")</f>
         <v/>
       </c>
-      <c r="F43" s="49"/>
-      <c r="G43" s="49"/>
+      <c r="F43" s="48"/>
+      <c r="G43" s="48"/>
     </row>
     <row r="44" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D44" s="1" t="str">
         <f>IF(AND(ISNUMBER(D43),D43&lt;B2),D43+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E44" s="58" t="str">
+      <c r="E44" s="57" t="str">
         <f>IF(ISNUMBER(D44),COMBIN(B2,D44)*B3^D44*(1-B3)^(B2-D44),"")</f>
         <v/>
       </c>
-      <c r="F44" s="49"/>
-      <c r="G44" s="49"/>
+      <c r="F44" s="48"/>
+      <c r="G44" s="48"/>
     </row>
     <row r="45" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D45" s="1" t="str">
         <f>IF(AND(ISNUMBER(D44),D44&lt;B2),D44+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E45" s="58" t="str">
+      <c r="E45" s="57" t="str">
         <f>IF(ISNUMBER(D45),COMBIN(B2,D45)*B3^D45*(1-B3)^(B2-D45),"")</f>
         <v/>
       </c>
-      <c r="F45" s="49"/>
-      <c r="G45" s="49"/>
+      <c r="F45" s="48"/>
+      <c r="G45" s="48"/>
     </row>
     <row r="46" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D46" s="1" t="str">
         <f>IF(AND(ISNUMBER(D45),D45&lt;B2),D45+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E46" s="58" t="str">
+      <c r="E46" s="57" t="str">
         <f>IF(ISNUMBER(D46),COMBIN(B2,D46)*B3^D46*(1-B3)^(B2-D46),"")</f>
         <v/>
       </c>
-      <c r="F46" s="49"/>
-      <c r="G46" s="49"/>
+      <c r="F46" s="48"/>
+      <c r="G46" s="48"/>
     </row>
     <row r="47" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D47" s="1" t="str">
         <f>IF(AND(ISNUMBER(D46),D46&lt;B2),D46+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E47" s="58" t="str">
+      <c r="E47" s="57" t="str">
         <f>IF(ISNUMBER(D47),COMBIN(B2,D47)*B3^D47*(1-B3)^(B2-D47),"")</f>
         <v/>
       </c>
-      <c r="F47" s="49"/>
-      <c r="G47" s="49"/>
+      <c r="F47" s="48"/>
+      <c r="G47" s="48"/>
     </row>
     <row r="48" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D48" s="1" t="str">
         <f>IF(AND(ISNUMBER(D47),D47&lt;B2),D47+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E48" s="58" t="str">
+      <c r="E48" s="57" t="str">
         <f>IF(ISNUMBER(D48),COMBIN(B2,D48)*B3^D48*(1-B3)^(B2-D48),"")</f>
         <v/>
       </c>
-      <c r="F48" s="49"/>
-      <c r="G48" s="49"/>
+      <c r="F48" s="48"/>
+      <c r="G48" s="48"/>
     </row>
     <row r="49" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D49" s="1" t="str">
         <f>IF(AND(ISNUMBER(D48),D48&lt;B2),D48+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E49" s="58" t="str">
+      <c r="E49" s="57" t="str">
         <f>IF(ISNUMBER(D49),COMBIN(B2,D49)*B3^D49*(1-B3)^(B2-D49),"")</f>
         <v/>
       </c>
-      <c r="F49" s="49"/>
-      <c r="G49" s="49"/>
+      <c r="F49" s="48"/>
+      <c r="G49" s="48"/>
     </row>
     <row r="50" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D50" s="1" t="str">
         <f>IF(AND(ISNUMBER(D49),D49&lt;B2),D49+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E50" s="58" t="str">
+      <c r="E50" s="57" t="str">
         <f>IF(ISNUMBER(D50),COMBIN(B2,D50)*B3^D50*(1-B3)^(B2-D50),"")</f>
         <v/>
       </c>
-      <c r="F50" s="49"/>
-      <c r="G50" s="49"/>
+      <c r="F50" s="48"/>
+      <c r="G50" s="48"/>
     </row>
     <row r="51" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D51" s="1" t="str">
         <f>IF(AND(ISNUMBER(D50),D50&lt;B2),D50+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E51" s="58" t="str">
+      <c r="E51" s="57" t="str">
         <f>IF(ISNUMBER(D51),COMBIN(B2,D51)*B3^D51*(1-B3)^(B2-D51),"")</f>
         <v/>
       </c>
-      <c r="F51" s="49"/>
-      <c r="G51" s="49"/>
+      <c r="F51" s="48"/>
+      <c r="G51" s="48"/>
     </row>
     <row r="52" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D52" s="1" t="str">
         <f>IF(AND(ISNUMBER(D51),D51&lt;B2),D51+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E52" s="58" t="str">
+      <c r="E52" s="57" t="str">
         <f>IF(ISNUMBER(D52),COMBIN(B2,D52)*B3^D52*(1-B3)^(B2-D52),"")</f>
         <v/>
       </c>
-      <c r="F52" s="49"/>
-      <c r="G52" s="49"/>
+      <c r="F52" s="48"/>
+      <c r="G52" s="48"/>
     </row>
     <row r="53" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D53" s="1" t="str">
         <f>IF(AND(ISNUMBER(D52),D52&lt;B2),D52+1," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E53" s="58" t="str">
+      <c r="E53" s="57" t="str">
         <f>IF(ISNUMBER(D53),COMBIN(B2,D53)*B3^D53*(1-B3)^(B2-D53),"")</f>
         <v/>
       </c>
-      <c r="F53" s="49"/>
-      <c r="G53" s="49"/>
+      <c r="F53" s="48"/>
+      <c r="G53" s="48"/>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
@@ -11270,6 +11103,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="EKin4zECxpgAsfKERZa+FX82ZIfQ7NfM65H1kTDmjl2rxvcC9l0WgpP/7G7LwL9VymzXRETL0/jJVQdLL7PKsA==" saltValue="b0EPrZsKYc0jHqD7LsdpUw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -11301,7 +11135,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="55" t="s">
         <v>63</v>
       </c>
       <c r="B2" s="40">
@@ -11309,7 +11143,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="55" t="s">
         <v>64</v>
       </c>
       <c r="B3" s="40">
@@ -11325,7 +11159,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="55" t="s">
         <v>57</v>
       </c>
       <c r="B6" s="40"/>
@@ -11334,7 +11168,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="55" t="s">
         <v>59</v>
       </c>
       <c r="B7" s="40"/>
@@ -11343,11 +11177,11 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="53" t="str">
+      <c r="A8" s="52" t="str">
         <f>CONCATENATE("P(", IF(ISBLANK(B6),"","lower ≤ "),IF(AND(B2=0,B3=1),"z","x"),IF(ISBLANK(B7),""," ≤ upper"),") =")</f>
         <v>P(z) =</v>
       </c>
-      <c r="B8" s="60" t="str">
+      <c r="B8" s="63" t="str">
         <f>IF(AND(ISBLANK(B6),ISBLANK(B7)),"",IF(OR(NOT(OR(ISBLANK(B6),ISNUMBER(B6))),NOT(OR(ISBLANK(B7),ISNUMBER(B7)))),"Input Error",IF(IF(OR(ISBLANK(B6),ISBLANK(B7)),FALSE,B6&gt;B7),"Input Error",IF(AND(ISNUMBER(B2),ISNUMBER(B3)),_xlfn.NORM.DIST(IF(ISBLANK(B7),1E+100,B7),B2,B3,TRUE)-_xlfn.NORM.DIST(IF(ISBLANK(B6),-1E+100,B6),B2,B3,TRUE),"Input µ,σ"))))</f>
         <v/>
       </c>
@@ -11362,21 +11196,21 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="59"/>
+      <c r="B11" s="58"/>
       <c r="C11" s="16" t="str">
         <f>IF(AND(B11&lt;1,B11&gt;=0),"","area must be between 0 and 1")</f>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="53" t="str">
+      <c r="A12" s="52" t="str">
         <f>IF(AND(B2=0,B3=1),"z =","x =")</f>
         <v>z =</v>
       </c>
-      <c r="B12" s="61" t="str">
+      <c r="B12" s="63" t="str">
         <f>IF(ISBLANK(B11),"",IF(NOT(ISNUMBER(B11)),"Input Error",IF(OR(B11&lt;=0,B11&gt;=1),"Input Error",IF(AND(ISNUMBER(B2),ISNUMBER(B3)),_xlfn.NORM.INV(B11,B2,B3),"Input µ,σ"))))</f>
         <v/>
       </c>
@@ -11390,7 +11224,9 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="Gu8kkGcGAD5OQ4F4aP2GOLh2/okVOCoB7Ux8zT9SGgFG88oQ++GDlIhc1IbMIWnC9ErHhVVU2KVU1ck/3k15iQ==" saltValue="g8LeosLKx6Wu5LXzYPSwOw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11420,7 +11256,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="55" t="s">
         <v>73</v>
       </c>
       <c r="B2" s="40"/>
@@ -11438,7 +11274,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="55" t="s">
         <v>57</v>
       </c>
       <c r="B5" s="40"/>
@@ -11447,7 +11283,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="55" t="s">
         <v>59</v>
       </c>
       <c r="B6" s="40"/>
@@ -11456,11 +11292,11 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="53" t="str">
+      <c r="A7" s="52" t="str">
         <f>CONCATENATE("P(", IF(ISBLANK(B5),"","lower ≤ "),"t",IF(ISBLANK(B6),""," ≤ upper"),") =")</f>
         <v>P(t) =</v>
       </c>
-      <c r="B7" s="57" t="str">
+      <c r="B7" s="63" t="str">
         <f>IF(AND(ISBLANK(B5),ISBLANK(B6)),"",IF(OR(NOT(OR(ISBLANK(B5),ISNUMBER(B5))),NOT(OR(ISBLANK(B6),ISNUMBER(B6)))),"Input Error",IF(IF(OR(ISBLANK(B5),ISBLANK(B6)),FALSE,B5&gt;B6),"Input Error",IF(B2&gt;0,IF(ISBLANK(B5),IF(B6&lt;0,TDIST(ABS(B6),B2,1),1-TDIST(ABS(B6),B2,1)),IF(ISBLANK(B6),IF(B5&lt;0,1-TDIST(ABS(B5),B2,1),TDIST(ABS(B5),B2,1)),IF(B5*B6&gt;=0,ABS(TDIST(ABS(B6),B2,1)-TDIST(ABS(B5),B2,1)),1-TDIST(ABS(B6),B2,1)-TDIST(ABS(B5),B2,1)))),"Input df"))))</f>
         <v/>
       </c>
@@ -11475,7 +11311,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="55" t="s">
         <v>70</v>
       </c>
       <c r="B10" s="40"/>
@@ -11485,10 +11321,10 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="38" t="str">
+      <c r="B11" s="63" t="str">
         <f>IF(ISBLANK(B10),"",IF(NOT(ISNUMBER(B10)),"Input Error",IF(OR(B10&lt;=0,B10&gt;=1),"Input Error",IF(B2&gt;0,_xlfn.T.INV(B10,B2),"Input df"))))</f>
         <v/>
       </c>
@@ -11502,6 +11338,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="QyRc6LuhJgxNt29Dd9G3sUBn7Z1Vo4sQbcpFolqzdckLwfW1plQqfY9sUEzm4h14XUZyxC6XLcsSffWov0ZtSQ==" saltValue="520A9H9BRZ3//hXhn3wjLw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -11695,6 +11532,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="g/L0+6Ohu4HU1I2hA2fmeuEmY4z9egIUTyfG/b5drpgLMOx/66x3hXnG0DGWmyGXn4RsiT1epz1lnyovWTyzoA==" saltValue="vvVtfcul3HS14g2wbi+9pQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -11762,7 +11600,7 @@
         <v>89</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C3" s="25" t="str">
         <f>IF(ISNUMBER(C2),C2,"")</f>
@@ -11871,7 +11709,7 @@
       <c r="B8" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="30" t="str">
+      <c r="C8" s="65" t="str">
         <f>IF(AND(ISNUMBER(C4),ISNUMBER(C5),ISNUMBER(C6),ISNUMBER(C2)),IF(AND(INT(C6)=C6,C6&gt;0,C5&gt;0),(C4-C2)/(C5/SQRT(C6)),"Input Error"),"")</f>
         <v/>
       </c>
@@ -11884,7 +11722,7 @@
       <c r="I8" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="30" t="str">
+      <c r="J8" s="65" t="str">
         <f>IF(AND(ISNUMBER(J2),ISNUMBER(J4),ISNUMBER(J5)),IF(AND(INT(J4)=J4,INT(J5)=J5,J2&gt;0,J2&lt;1,J5&gt;0,J5&lt;J4),(J6-J2)/SQRT(J2*(1-J2)/J4),"Input Error"),"")</f>
         <v/>
       </c>
@@ -11899,7 +11737,7 @@
       <c r="B9" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="30" t="str">
+      <c r="C9" s="65" t="str">
         <f>IF(AND(ISNUMBER(C4),ISNUMBER(C5),ISNUMBER(C6),ISNUMBER(C2)),IF(AND(INT(C6)=C6,C6&gt;0,C5&gt;0),IF(B3="≠",2*IF(C8&lt;0,NORMSDIST(C8),1-NORMSDIST(C8)),IF(B3="&lt;",NORMSDIST(C8),IF(B3="&gt;",1-NORMSDIST(C8),"Select H1"))),"Input Error"),"")</f>
         <v/>
       </c>
@@ -11912,7 +11750,7 @@
       <c r="I9" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="30" t="str">
+      <c r="J9" s="65" t="str">
         <f>IF(AND(ISNUMBER(J2),ISNUMBER(J4),ISNUMBER(J5)),IF(AND(INT(J4)=J4,INT(J5)=J5,J2&gt;0,J2&lt;1,J5&gt;0,J5&lt;J4),IF(I3="≠",2*IF(J8&lt;0,NORMSDIST(J8),1-NORMSDIST(J8)),IF(I3="&lt;",NORMSDIST(J8),IF(I3="&gt;",1-NORMSDIST(J8),"Select H1"))),"Input Error"),"")</f>
         <v/>
       </c>
@@ -12002,7 +11840,7 @@
       <c r="B18" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="30" t="str">
+      <c r="C18" s="65" t="str">
         <f>IF(AND(ISNUMBER(C14),ISNUMBER(C15),ISNUMBER(C16),ISNUMBER(C12)),IF(AND(INT(C16)=C16,C16&gt;0,C15&gt;0),(C14-C12)/(C15/SQRT(C16)),"Input Error"),"")</f>
         <v/>
       </c>
@@ -12017,7 +11855,7 @@
       <c r="B19" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="30" t="str">
+      <c r="C19" s="65" t="str">
         <f>IF(AND(ISNUMBER(C14),ISNUMBER(C15),ISNUMBER(C16),ISNUMBER(C12)),IF(AND(INT(C16)=C16,C16&gt;0,C15&gt;0),IF(B13="≠",TDIST(ABS(C18),C16-1,2),IF(B13="&lt;",IF(C18&lt;0,TDIST(ABS(C18),C16-1,1),1-TDIST(ABS(C18),C16-1,1)),IF(B13="&gt;",IF(C18&lt;0,1-TDIST(ABS(C18),C16-1,1),TDIST(ABS(C18),C16-1,1)),"Select H1"))),"Input Error"),"")</f>
         <v/>
       </c>
@@ -12049,6 +11887,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="FAXMHmEmyMnqjXgYIqFq9K1c9Gtn1SUyZGJv7aFc4E2FwMG5kY4atfAXtTBYhkSgngXMlUfAfUDChdppicbV/g==" saltValue="BHHojX6RJVv1zbsJm1K2SA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataValidations xWindow="100" yWindow="336" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select H1" prompt="≠, &lt;, or &gt;" sqref="B3 I3 B13" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>$A$98:$A$100</formula1>
@@ -12128,7 +11967,7 @@
         <v>108</v>
       </c>
       <c r="I3" s="42" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J3" s="32" t="s">
         <v>106</v>
@@ -12290,7 +12129,7 @@
       <c r="B11" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="30" t="str">
+      <c r="C11" s="65" t="str">
         <f>IF(AND(ISNUMBER(C4),ISNUMBER(C5),ISNUMBER(C6),ISNUMBER(C7),ISNUMBER(C8),ISNUMBER(C9)),IF(AND(INT(C6)=C6,C6&gt;0,C5&gt;0,INT(C9)=C9,C9&gt;0,C8&gt;0),(C4-C7)/SQRT(C5^2/C6+C8^2/C9),"Input Error"),"")</f>
         <v/>
       </c>
@@ -12303,7 +12142,7 @@
       <c r="I11" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J11" s="30" t="str">
+      <c r="J11" s="65" t="str">
         <f>IF(AND(ISNUMBER(J4),ISNUMBER(J5),ISNUMBER(J7),ISNUMBER(J8)),IF(AND(INT(J4)=J4,INT(J5)=J5,J5&gt;0,J5&lt;J4,INT(J7)=J7,INT(J8)=J8,J8&gt;0,J8&lt;J7),(J6-J9)/SQRT(((J5+J8)/(J4+J7))*(1-((J5+J8)/(J4+J7)))/J4+((J5+J8)/(J4+J7))*(1-((J5+J8)/(J4+J7)))/J7),"Input Error"),"")</f>
         <v/>
       </c>
@@ -12331,7 +12170,7 @@
       <c r="I12" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J12" s="30" t="str">
+      <c r="J12" s="65" t="str">
         <f>IF(AND(ISNUMBER(J4),ISNUMBER(J5),ISNUMBER(J7),ISNUMBER(J8)),IF(AND(INT(J4)=J4,INT(J5)=J5,J5&gt;0,J5&lt;J4,INT(J7)=J7,INT(J8)=J8,J8&gt;0,J8&lt;J7),IF(I3="≠",2*IF(J11&lt;0,NORMSDIST(J11),1-NORMSDIST(J11)),IF(I3="&lt;",NORMSDIST(J11),IF(I3="&gt;",1-NORMSDIST(J11),"Select H1"))),"Input Error"),"")</f>
         <v/>
       </c>
@@ -12346,7 +12185,7 @@
       <c r="B13" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="30" t="str">
+      <c r="C13" s="65" t="str">
         <f>IF(AND(ISNUMBER(C4),ISNUMBER(C5),ISNUMBER(C6),ISNUMBER(C7),ISNUMBER(C8),ISNUMBER(C9)),IF(AND(INT(C6)=C6,C6&gt;0,C5&gt;0,INT(C9)=C9,C9&gt;0,C8&gt;0), IF(B3="≠",TDIST(ABS(C11),C12,2),IF(B3="&lt;",IF(C11&lt;0,TDIST(ABS(C11),C12,1),1-TDIST(ABS(C11),C12,1)),IF(B3="&gt;",IF(C11&lt;0,1-TDIST(ABS(C11),C12,1),TDIST(ABS(C11),C12,1)),"Select H1"))),"Input Error"),"")</f>
         <v/>
       </c>
@@ -12375,6 +12214,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="jKyu0cRiy3HXbGiLACOA0xTk5Qx4CofzkQ/F6akIyQqW30KM8BeJkTnaueppshVaCgaVJ4Js9/Fx5oI5PA2fWg==" saltValue="xk6kzGKKtPamGzJr1+ddNQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select H1" prompt="≠, &lt;, or &gt;" sqref="B3 I3" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>$A$93:$A$95</formula1>

</xml_diff>